<commit_message>
fix for attribute error in personalInfo if only 1 parameter is passed
</commit_message>
<xml_diff>
--- a/excel_files/testdata.xlsx
+++ b/excel_files/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\manageLife-fsa-pageObject-scripts\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1121BC45-3C27-490A-9BDA-A4DADE53BCDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B1B480-3ADB-4524-9B20-7BBD527BB299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1710" windowWidth="24930" windowHeight="13395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
@@ -38,12 +38,6 @@
   </si>
   <si>
     <t>middlename</t>
-  </si>
-  <si>
-    <t>zipcode</t>
-  </si>
-  <si>
-    <t>ziptest</t>
   </si>
   <si>
     <t>dave</t>
@@ -409,10 +403,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6388700-2646-439E-B2E7-ADA147ED4D2C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,20 +414,14 @@
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>